<commit_message>
updated system on 2024-01-31
</commit_message>
<xml_diff>
--- a/admin/assets/uploads/add_student.xlsx
+++ b/admin/assets/uploads/add_student.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="58">
   <si>
     <t>Applicant Number</t>
   </si>
@@ -67,18 +67,9 @@
     <t>Disability Type</t>
   </si>
   <si>
-    <t>Institution Code</t>
-  </si>
-  <si>
     <t>Application Type</t>
   </si>
   <si>
-    <t>Programme Applied Code</t>
-  </si>
-  <si>
-    <t>Programme Offered Code</t>
-  </si>
-  <si>
     <t>Admission Year</t>
   </si>
   <si>
@@ -94,16 +85,16 @@
     <t>Fee Payment Type</t>
   </si>
   <si>
-    <t>UPS/2022/0074</t>
-  </si>
-  <si>
-    <t>Hannah</t>
+    <t>KST/2022/0067</t>
+  </si>
+  <si>
+    <t>Gloria</t>
   </si>
   <si>
     <t>Johnson</t>
   </si>
   <si>
-    <t>Ashiokai</t>
+    <t>Ansah</t>
   </si>
   <si>
     <t>Female</t>
@@ -139,17 +130,6 @@
     <t>No</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>UPS/001/0004</t>
-    </r>
-  </si>
-  <si>
     <t>Undergraduate</t>
   </si>
   <si>
@@ -162,13 +142,13 @@
     <t>Full Fee-Paying</t>
   </si>
   <si>
-    <t>UG/2020/053</t>
-  </si>
-  <si>
-    <t>Moses</t>
-  </si>
-  <si>
-    <t>Yankson</t>
+    <t>KST/2020/053</t>
+  </si>
+  <si>
+    <t>Mustapha</t>
+  </si>
+  <si>
+    <t>Mummin</t>
   </si>
   <si>
     <t>Male</t>
@@ -183,9 +163,6 @@
     <t>Togolese</t>
   </si>
   <si>
-    <t>Togo</t>
-  </si>
-  <si>
     <t>Moslem</t>
   </si>
   <si>
@@ -205,9 +182,6 @@
   </si>
   <si>
     <t>Eye</t>
-  </si>
-  <si>
-    <t>UG0010</t>
   </si>
   <si>
     <t>regular</t>
@@ -227,7 +201,7 @@
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -378,12 +352,6 @@
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1157,10 +1125,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2"/>
@@ -1182,18 +1150,15 @@
     <col min="15" max="15" width="19.5555555555556" style="1" customWidth="1"/>
     <col min="16" max="16" width="15" customWidth="1"/>
     <col min="17" max="17" width="13.7777777777778" customWidth="1"/>
-    <col min="18" max="18" width="15.2222222222222" customWidth="1"/>
-    <col min="19" max="19" width="15.7777777777778" customWidth="1"/>
-    <col min="20" max="20" width="23.7777777777778" customWidth="1"/>
-    <col min="21" max="21" width="24.1111111111111" customWidth="1"/>
-    <col min="22" max="22" width="14.5555555555556" customWidth="1"/>
-    <col min="23" max="23" width="16.1111111111111" customWidth="1"/>
-    <col min="24" max="24" width="17" customWidth="1"/>
-    <col min="25" max="25" width="17.1111111111111" customWidth="1"/>
-    <col min="26" max="26" width="17.2222222222222" customWidth="1"/>
+    <col min="18" max="18" width="15.7777777777778" customWidth="1"/>
+    <col min="19" max="19" width="14.5555555555556" customWidth="1"/>
+    <col min="20" max="20" width="16.1111111111111" customWidth="1"/>
+    <col min="21" max="21" width="17" customWidth="1"/>
+    <col min="22" max="22" width="17.1111111111111" customWidth="1"/>
+    <col min="23" max="23" width="17.2222222222222" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:23">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1263,168 +1228,141 @@
       <c r="W1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+    </row>
+    <row r="2" spans="1:23">
+      <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="B2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="C2" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:26">
-      <c r="A2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="E2" s="2">
         <v>23833</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="P2" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="R2" t="s">
         <v>38</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="S2">
+        <v>2022</v>
+      </c>
+      <c r="T2" t="s">
         <v>39</v>
       </c>
-      <c r="P2" t="s">
+      <c r="U2" t="s">
         <v>40</v>
       </c>
-      <c r="R2" t="s">
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2" t="s">
         <v>41</v>
       </c>
-      <c r="S2" t="s">
+    </row>
+    <row r="3" spans="1:23">
+      <c r="A3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="T2">
-        <v>16</v>
-      </c>
-      <c r="U2">
-        <v>16</v>
-      </c>
-      <c r="V2">
-        <v>2022</v>
-      </c>
-      <c r="W2" t="s">
+      <c r="B3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="X2" t="s">
+      <c r="C3" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="Y2">
-        <v>1</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26">
-      <c r="A3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="E3" s="2">
         <v>28551</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="P3" t="s">
         <v>54</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="Q3" t="s">
         <v>55</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="R3" t="s">
+        <v>38</v>
+      </c>
+      <c r="S3">
+        <v>2020</v>
+      </c>
+      <c r="T3" t="s">
         <v>56</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="U3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+      <c r="W3" t="s">
         <v>57</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="P3" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>60</v>
-      </c>
-      <c r="R3" t="s">
-        <v>61</v>
-      </c>
-      <c r="S3" t="s">
-        <v>42</v>
-      </c>
-      <c r="T3">
-        <v>15</v>
-      </c>
-      <c r="U3">
-        <v>15</v>
-      </c>
-      <c r="V3">
-        <v>2020</v>
-      </c>
-      <c r="W3" t="s">
-        <v>62</v>
-      </c>
-      <c r="X3" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y3">
-        <v>1</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1441,16 +1379,16 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P1:P3 P4:P1048576">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S1:S3 S4:S1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R1:R3 R4:R1048576">
       <formula1>"Undergraduate,Postgraduate,International"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W1:W3 W4:W1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T1:T3 T4:T1048576">
       <formula1>"distance,evening,regular,weekend"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X1:X3 X4:X1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U1:U3 U4:U1048576">
       <formula1>"Qualified,Offered,Enrolled,Graduated"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z1:Z3 Z4:Z1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W1:W3 W4:W1048576">
       <formula1>"Full Fee-Paying, Government Subsidized, Scholarship"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>